<commit_message>
PLaying around with the auto plots a little
</commit_message>
<xml_diff>
--- a/CustomPlots/attitude_tuning.xlsx
+++ b/CustomPlots/attitude_tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24AD1E9-A0A7-4884-97F3-2B04B8CFB48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A660BAD-EE4F-40D7-8341-30B9033015E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>KSID Custom Plot Definition</t>
   </si>
@@ -165,16 +165,22 @@
     <t>ATT/Yaw</t>
   </si>
   <si>
-    <t>POS/RelOriginAlt</t>
-  </si>
-  <si>
     <t>Attitude Tuning</t>
   </si>
   <si>
     <t>CTUN/DSAlt</t>
   </si>
   <si>
-    <t>Des Alt</t>
+    <t>CTUN/Alt</t>
+  </si>
+  <si>
+    <t>CTUN/SAlt</t>
+  </si>
+  <si>
+    <t>Sonar Altitude</t>
+  </si>
+  <si>
+    <t>Des Altitude</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -576,7 +582,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <f>1920-200</f>
@@ -876,7 +882,7 @@
         <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -911,15 +917,50 @@
         <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>49</v>
+      </c>
+      <c r="S14" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improving the custom plots
</commit_message>
<xml_diff>
--- a/CustomPlots/attitude_tuning.xlsx
+++ b/CustomPlots/attitude_tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A660BAD-EE4F-40D7-8341-30B9033015E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C369A6-71EC-41A4-BCD9-84A0DC06D971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
@@ -165,12 +165,6 @@
     <t>ATT/Yaw</t>
   </si>
   <si>
-    <t>Attitude Tuning</t>
-  </si>
-  <si>
-    <t>CTUN/DSAlt</t>
-  </si>
-  <si>
     <t>CTUN/Alt</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>Des Altitude</t>
+  </si>
+  <si>
+    <t>CTUN/DAlt</t>
+  </si>
+  <si>
+    <t>AttitudeTuning</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <f>1920-200</f>
@@ -882,7 +882,7 @@
         <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -917,13 +917,13 @@
         <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S13" t="s">
         <v>26</v>
@@ -952,13 +952,13 @@
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S14" t="s">
         <v>26</v>

</xml_diff>